<commit_message>
Add MR series (MR9000) Script
</commit_message>
<xml_diff>
--- a/CyberRouterATE/bin/Debug/testCondition/FwStress/FwStressFinalTestItems.xlsx
+++ b/CyberRouterATE/bin/Debug/testCondition/FwStress/FwStressFinalTestItems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="225" windowWidth="10245" windowHeight="7755"/>
+    <workbookView xWindow="-12" yWindow="288" windowWidth="10248" windowHeight="7692"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,19 +474,19 @@
   <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="5"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
-    <col min="5" max="9" width="10.75" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
+    <col min="5" max="9" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -515,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="str">
         <f>IF(E2&lt;&gt;"",ROW(B2),"")</f>
         <v/>
@@ -529,7 +529,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -546,10 +546,10 @@
         <v>11</v>
       </c>
       <c r="F3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -566,13 +566,13 @@
         <v>21</v>
       </c>
       <c r="F4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1</v>
       </c>
@@ -586,10 +586,10 @@
         <v>21</v>
       </c>
       <c r="F6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2</v>
       </c>
@@ -603,10 +603,10 @@
         <v>11</v>
       </c>
       <c r="F7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -617,7 +617,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -628,7 +628,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -639,7 +639,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -650,7 +650,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -661,7 +661,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -672,7 +672,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
@@ -683,7 +683,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
@@ -694,7 +694,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -705,7 +705,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -716,7 +716,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
@@ -727,7 +727,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
@@ -738,7 +738,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
@@ -749,7 +749,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
@@ -760,7 +760,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
@@ -771,7 +771,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
@@ -782,7 +782,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
@@ -793,7 +793,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
@@ -804,7 +804,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
@@ -815,7 +815,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
@@ -826,7 +826,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
@@ -837,7 +837,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
@@ -848,7 +848,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
@@ -859,7 +859,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
@@ -870,7 +870,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
@@ -881,7 +881,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
@@ -892,7 +892,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
@@ -903,7 +903,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
@@ -914,7 +914,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
@@ -925,7 +925,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
@@ -936,7 +936,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
@@ -947,7 +947,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
@@ -958,7 +958,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -969,7 +969,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
@@ -980,7 +980,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
@@ -991,7 +991,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -1002,7 +1002,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
@@ -1013,7 +1013,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
@@ -1024,7 +1024,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
@@ -1035,7 +1035,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
@@ -1046,7 +1046,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
@@ -1057,7 +1057,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
@@ -1068,7 +1068,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
@@ -1079,7 +1079,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
@@ -1090,7 +1090,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
@@ -1101,7 +1101,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
@@ -1112,7 +1112,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
@@ -1123,7 +1123,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
@@ -1134,7 +1134,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
@@ -1145,7 +1145,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="2"/>
       <c r="C57" s="3"/>
@@ -1156,7 +1156,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="2"/>
       <c r="C58" s="3"/>
@@ -1167,7 +1167,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="2"/>
       <c r="C59" s="3"/>
@@ -1178,7 +1178,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
@@ -1189,7 +1189,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="2"/>
       <c r="C61" s="3"/>
@@ -1200,7 +1200,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="2"/>
       <c r="C62" s="3"/>
@@ -1211,7 +1211,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="2"/>
       <c r="C63" s="3"/>
@@ -1222,7 +1222,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="2"/>
       <c r="C64" s="3"/>
@@ -1233,7 +1233,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="2"/>
       <c r="C65" s="3"/>
@@ -1244,7 +1244,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="2"/>
       <c r="C66" s="3"/>
@@ -1255,7 +1255,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="2"/>
       <c r="C67" s="3"/>
@@ -1266,7 +1266,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="2"/>
       <c r="C68" s="3"/>
@@ -1277,7 +1277,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="2"/>
       <c r="C69" s="3"/>
@@ -1288,7 +1288,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="2"/>
       <c r="C70" s="3"/>
@@ -1299,7 +1299,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="2"/>
       <c r="C71" s="3"/>
@@ -1310,7 +1310,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="2"/>
       <c r="C72" s="3"/>
@@ -1321,7 +1321,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="2"/>
       <c r="C73" s="3"/>
@@ -1332,7 +1332,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="2"/>
       <c r="C74" s="3"/>
@@ -1343,7 +1343,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="2"/>
       <c r="C75" s="3"/>
@@ -1354,7 +1354,7 @@
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="2"/>
       <c r="C76" s="3"/>
@@ -1365,7 +1365,7 @@
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="2"/>
       <c r="C77" s="3"/>
@@ -1376,7 +1376,7 @@
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="2"/>
       <c r="C78" s="3"/>
@@ -1387,7 +1387,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="2"/>
       <c r="C79" s="3"/>
@@ -1398,7 +1398,7 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="2"/>
       <c r="C80" s="3"/>
@@ -1409,7 +1409,7 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="2"/>
       <c r="C81" s="3"/>
@@ -1420,7 +1420,7 @@
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="2"/>
       <c r="C82" s="3"/>
@@ -1431,7 +1431,7 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="2"/>
       <c r="C83" s="3"/>
@@ -1442,7 +1442,7 @@
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="2"/>
       <c r="C84" s="3"/>
@@ -1453,7 +1453,7 @@
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
@@ -1464,7 +1464,7 @@
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="2"/>
       <c r="C86" s="3"/>
@@ -1475,7 +1475,7 @@
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="2"/>
       <c r="C87" s="3"/>
@@ -1486,7 +1486,7 @@
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="2"/>
       <c r="C88" s="3"/>
@@ -1497,7 +1497,7 @@
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="2"/>
       <c r="C89" s="3"/>
@@ -1508,7 +1508,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="2"/>
       <c r="C90" s="3"/>
@@ -1519,7 +1519,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="2"/>
       <c r="C91" s="3"/>
@@ -1530,7 +1530,7 @@
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="2"/>
       <c r="C92" s="3"/>
@@ -1541,7 +1541,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="2"/>
       <c r="C93" s="3"/>
@@ -1552,7 +1552,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="2"/>
       <c r="C94" s="3"/>
@@ -1563,7 +1563,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="2"/>
       <c r="C95" s="3"/>
@@ -1574,7 +1574,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="2"/>
       <c r="C96" s="3"/>
@@ -1585,7 +1585,7 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="2"/>
       <c r="C97" s="3"/>
@@ -1596,7 +1596,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="2"/>
       <c r="C98" s="3"/>
@@ -1607,7 +1607,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="2"/>
       <c r="C99" s="3"/>
@@ -1618,7 +1618,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="2"/>
       <c r="C100" s="3"/>
@@ -1629,7 +1629,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="2"/>
       <c r="C101" s="3"/>
@@ -1640,7 +1640,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="2"/>
       <c r="C102" s="3"/>
@@ -1651,7 +1651,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="2"/>
       <c r="C103" s="3"/>
@@ -1662,7 +1662,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="2"/>
       <c r="C104" s="3"/>
@@ -1673,7 +1673,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="2"/>
       <c r="C105" s="3"/>
@@ -1684,7 +1684,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="2"/>
       <c r="C106" s="3"/>
@@ -1695,7 +1695,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="2"/>
       <c r="C107" s="3"/>
@@ -1706,7 +1706,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
       <c r="B108" s="2"/>
       <c r="C108" s="3"/>
@@ -1717,7 +1717,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
       <c r="B109" s="2"/>
       <c r="C109" s="3"/>
@@ -1728,7 +1728,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="2"/>
       <c r="C110" s="3"/>
@@ -1739,7 +1739,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="2"/>
       <c r="C111" s="3"/>
@@ -1750,7 +1750,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="2"/>
       <c r="C112" s="3"/>
@@ -1761,7 +1761,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="2"/>
       <c r="C113" s="3"/>
@@ -1772,7 +1772,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="2"/>
       <c r="C114" s="3"/>
@@ -1783,7 +1783,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
       <c r="B115" s="2"/>
       <c r="C115" s="3"/>
@@ -1794,7 +1794,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
       <c r="B116" s="2"/>
       <c r="C116" s="3"/>
@@ -1805,7 +1805,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
       <c r="B117" s="2"/>
       <c r="C117" s="3"/>
@@ -1816,7 +1816,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="6"/>
       <c r="B118" s="2"/>
       <c r="C118" s="3"/>
@@ -1827,7 +1827,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
       <c r="B119" s="2"/>
       <c r="C119" s="3"/>
@@ -1838,7 +1838,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
       <c r="B120" s="2"/>
       <c r="C120" s="3"/>
@@ -1849,7 +1849,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
       <c r="B121" s="2"/>
       <c r="C121" s="3"/>
@@ -1860,7 +1860,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="6"/>
       <c r="B122" s="2"/>
       <c r="C122" s="3"/>
@@ -1871,7 +1871,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
       <c r="B123" s="2"/>
       <c r="C123" s="3"/>
@@ -1882,7 +1882,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="6"/>
       <c r="B124" s="2"/>
       <c r="C124" s="3"/>
@@ -1893,7 +1893,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
       <c r="B125" s="2"/>
       <c r="C125" s="3"/>
@@ -1904,7 +1904,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
       <c r="B126" s="2"/>
       <c r="C126" s="3"/>
@@ -1915,7 +1915,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
       <c r="B127" s="2"/>
       <c r="C127" s="3"/>
@@ -1926,7 +1926,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
       <c r="B128" s="2"/>
       <c r="C128" s="3"/>
@@ -1937,7 +1937,7 @@
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
       <c r="B129" s="2"/>
       <c r="C129" s="3"/>
@@ -1948,7 +1948,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
       <c r="B130" s="2"/>
       <c r="C130" s="3"/>
@@ -1974,7 +1974,7 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>